<commit_message>
Training for 9 cubes with 6-7 letter words
</commit_message>
<xml_diff>
--- a/Evaluation/stat1.xlsx
+++ b/Evaluation/stat1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\E-MaxPCShop\PycharmProjects\LetterCubicGame\Evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0B2BB9-93E9-49FD-BBD6-FBB370DD2D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CC89C3-9869-419C-9634-91A22EEF6BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="735" xr2:uid="{959A09F0-7163-4691-A974-626E1E6A92F8}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="79">
   <si>
     <r>
       <t> </t>
@@ -314,6 +314,12 @@
   <si>
     <t># test+train words</t>
   </si>
+  <si>
+    <t>6 letter</t>
+  </si>
+  <si>
+    <t>7 letter</t>
+  </si>
 </sst>
 </file>
 
@@ -445,7 +451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -494,34 +500,22 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -530,14 +524,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -905,42 +914,43 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="10" width="7.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="29"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="30"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="33"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="29"/>
       <c r="D2" s="10" t="s">
         <v>23</v>
       </c>
@@ -967,34 +977,34 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="26" t="s">
         <v>74</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="37">
         <v>69.5</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="37">
         <v>68.7</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="37">
         <v>0.95131487952202398</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="37">
         <v>79.179000000000002</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="37">
         <v>1.6984643063661899</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="37">
         <v>61.188600000000001</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3" s="37">
         <v>1.8764838928165599</v>
       </c>
       <c r="K3">
@@ -1002,30 +1012,30 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="31"/>
-      <c r="B4" s="35"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="26"/>
       <c r="C4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="37">
         <v>57.1</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="37">
         <v>55.78</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="37">
         <v>0.84675852520066297</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="37">
         <v>66.233199999999997</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="37">
         <v>1.2959366111041</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="37">
         <v>48.3</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="37">
         <v>1.1886317764556</v>
       </c>
       <c r="K4">
@@ -1033,232 +1043,232 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>72</v>
+      <c r="A5" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="10">
-        <v>57.5</v>
-      </c>
-      <c r="E5" s="10">
-        <v>56.3</v>
-      </c>
-      <c r="F5" s="10">
-        <v>1.0271319292087</v>
-      </c>
-      <c r="G5" s="10">
-        <v>69.053600000000003</v>
-      </c>
-      <c r="H5" s="10">
-        <v>1.34823321424744</v>
-      </c>
-      <c r="I5" s="10">
-        <v>48.100200000000001</v>
-      </c>
-      <c r="J5" s="10">
-        <v>1.4569099834924599</v>
+      <c r="D5" s="37">
+        <v>74.5</v>
+      </c>
+      <c r="E5" s="37">
+        <v>74.239999999999995</v>
+      </c>
+      <c r="F5" s="37">
+        <v>0.19493588689617899</v>
+      </c>
+      <c r="G5" s="37">
+        <v>83.453599999999994</v>
+      </c>
+      <c r="H5" s="37">
+        <v>0.73452794364816199</v>
+      </c>
+      <c r="I5" s="37">
+        <v>66.810199999999995</v>
+      </c>
+      <c r="J5" s="37">
+        <v>0.98428537528503401</v>
       </c>
       <c r="K5">
-        <v>0.27857446670532199</v>
+        <v>0.34156870841979903</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="31"/>
-      <c r="B6" s="31"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="10">
-        <v>84.5</v>
-      </c>
-      <c r="E6" s="10">
-        <v>83.88</v>
-      </c>
-      <c r="F6" s="10">
-        <v>0.540370243444253</v>
-      </c>
-      <c r="G6" s="10">
-        <v>90.755200000000002</v>
-      </c>
-      <c r="H6" s="10">
-        <v>0.62236862067427901</v>
-      </c>
-      <c r="I6" s="10">
-        <v>79.486199999999997</v>
-      </c>
-      <c r="J6" s="10">
-        <v>0.60873820317111704</v>
+      <c r="D6" s="37">
+        <v>81.8</v>
+      </c>
+      <c r="E6" s="37">
+        <v>81.28</v>
+      </c>
+      <c r="F6" s="37">
+        <v>0.55407580708780102</v>
+      </c>
+      <c r="G6" s="37">
+        <v>88.380399999999995</v>
+      </c>
+      <c r="H6" s="37">
+        <v>0.662934612160203</v>
+      </c>
+      <c r="I6" s="37">
+        <v>75.5852</v>
+      </c>
+      <c r="J6" s="37">
+        <v>1.56171418639903</v>
       </c>
       <c r="K6">
-        <v>0.22135424613952601</v>
+        <v>0.37186455726623502</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="31" t="s">
-        <v>71</v>
+      <c r="A7" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>72</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="10">
-        <v>57.9</v>
-      </c>
-      <c r="E7" s="10">
-        <v>56.699999999999903</v>
-      </c>
-      <c r="F7" s="10">
-        <v>1.0198039027185499</v>
-      </c>
-      <c r="G7" s="10">
-        <v>68.175200000000004</v>
-      </c>
-      <c r="H7" s="10">
-        <v>1.58167496660976</v>
-      </c>
-      <c r="I7" s="10">
-        <v>48.192599999999999</v>
-      </c>
-      <c r="J7" s="10">
-        <v>1.5771342048157999</v>
+      <c r="D7" s="37">
+        <v>57.5</v>
+      </c>
+      <c r="E7" s="37">
+        <v>56.3</v>
+      </c>
+      <c r="F7" s="37">
+        <v>1.0271319292087</v>
+      </c>
+      <c r="G7" s="37">
+        <v>69.053600000000003</v>
+      </c>
+      <c r="H7" s="37">
+        <v>1.34823321424744</v>
+      </c>
+      <c r="I7" s="37">
+        <v>48.100200000000001</v>
+      </c>
+      <c r="J7" s="37">
+        <v>1.4569099834924599</v>
       </c>
       <c r="K7">
-        <v>0.38980340957641602</v>
+        <v>0.27857446670532199</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="31"/>
-      <c r="B8" s="31"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
       <c r="C8" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="10">
-        <v>42.1</v>
-      </c>
-      <c r="E8" s="10">
-        <v>40.78</v>
-      </c>
-      <c r="F8" s="10">
-        <v>0.82280009722896796</v>
-      </c>
-      <c r="G8" s="10">
-        <v>51.567399999999999</v>
-      </c>
-      <c r="H8" s="10">
-        <v>1.47763892747856</v>
-      </c>
-      <c r="I8" s="10">
-        <v>32.816600000000001</v>
-      </c>
-      <c r="J8" s="10">
-        <v>0.45481347825234802</v>
+      <c r="D8" s="37">
+        <v>84.5</v>
+      </c>
+      <c r="E8" s="37">
+        <v>83.88</v>
+      </c>
+      <c r="F8" s="37">
+        <v>0.540370243444253</v>
+      </c>
+      <c r="G8" s="37">
+        <v>90.755200000000002</v>
+      </c>
+      <c r="H8" s="37">
+        <v>0.62236862067427901</v>
+      </c>
+      <c r="I8" s="37">
+        <v>79.486199999999997</v>
+      </c>
+      <c r="J8" s="37">
+        <v>0.60873820317111704</v>
       </c>
       <c r="K8">
-        <v>0.441425800323486</v>
+        <v>0.22135424613952601</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>70</v>
+      <c r="A9" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>71</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="10">
-        <v>42</v>
-      </c>
-      <c r="E9" s="10">
-        <v>41.7</v>
-      </c>
-      <c r="F9" s="10">
-        <v>0.367423461417476</v>
-      </c>
-      <c r="G9" s="10">
-        <v>52.542999999999999</v>
-      </c>
-      <c r="H9" s="10">
-        <v>1.12343936195951</v>
-      </c>
-      <c r="I9" s="10">
-        <v>34.295000000000002</v>
-      </c>
-      <c r="J9" s="10">
-        <v>0.30798782443466599</v>
+      <c r="D9" s="37">
+        <v>57.9</v>
+      </c>
+      <c r="E9" s="37">
+        <v>56.699999999999903</v>
+      </c>
+      <c r="F9" s="37">
+        <v>1.0198039027185499</v>
+      </c>
+      <c r="G9" s="37">
+        <v>68.175200000000004</v>
+      </c>
+      <c r="H9" s="37">
+        <v>1.58167496660976</v>
+      </c>
+      <c r="I9" s="37">
+        <v>48.192599999999999</v>
+      </c>
+      <c r="J9" s="37">
+        <v>1.5771342048157999</v>
       </c>
       <c r="K9">
-        <v>1.04804134368896</v>
+        <v>0.38980340957641602</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="31"/>
-      <c r="B10" s="31"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="10">
-        <v>25.6</v>
-      </c>
-      <c r="E10" s="10">
-        <v>24.64</v>
-      </c>
-      <c r="F10" s="10">
-        <v>0.832466215530696</v>
-      </c>
-      <c r="G10" s="10">
-        <v>35.057000000000002</v>
-      </c>
-      <c r="H10" s="10">
-        <v>1.72089453482774</v>
-      </c>
-      <c r="I10" s="10">
-        <v>17.461600000000001</v>
-      </c>
-      <c r="J10" s="10">
-        <v>0.35255680393377598</v>
+      <c r="D10" s="37">
+        <v>42.1</v>
+      </c>
+      <c r="E10" s="37">
+        <v>40.78</v>
+      </c>
+      <c r="F10" s="37">
+        <v>0.82280009722896796</v>
+      </c>
+      <c r="G10" s="37">
+        <v>51.567399999999999</v>
+      </c>
+      <c r="H10" s="37">
+        <v>1.47763892747856</v>
+      </c>
+      <c r="I10" s="37">
+        <v>32.816600000000001</v>
+      </c>
+      <c r="J10" s="37">
+        <v>0.45481347825234802</v>
       </c>
       <c r="K10">
-        <v>0.81218218803405695</v>
+        <v>0.441425800323486</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="23" t="s">
         <v>69</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="37">
         <v>76.2</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="37">
         <v>74.180000000000007</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="37">
         <v>1.22759928315391</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="37">
         <v>84.7196</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="37">
         <v>0.36859096570588401</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="37">
         <v>66.250600000000006</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="37">
         <v>1.97040561814059</v>
       </c>
       <c r="K11">
@@ -1266,30 +1276,30 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="31"/>
-      <c r="B12" s="31"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="23"/>
       <c r="C12" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="37">
         <v>84.5</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="37">
         <v>83.6</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="37">
         <v>0.77781745930520396</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="37">
         <v>91.533000000000001</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12" s="37">
         <v>0.59921281695237305</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="37">
         <v>77.597200000000001</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="37">
         <v>1.4583028492051899</v>
       </c>
       <c r="K12">
@@ -1297,34 +1307,34 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="23" t="s">
         <v>68</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="37">
         <v>65.3</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="37">
         <v>64.42</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="37">
         <v>0.90939540355116999</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="37">
         <v>76.334000000000003</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13" s="37">
         <v>1.07462830783485</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="37">
         <v>56.284599999999998</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="37">
         <v>1.12609027169228</v>
       </c>
       <c r="K13">
@@ -1332,30 +1342,30 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="31"/>
-      <c r="B14" s="31"/>
+      <c r="A14" s="23"/>
+      <c r="B14" s="23"/>
       <c r="C14" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="37">
         <v>54.2</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="37">
         <v>53</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="37">
         <v>1.0606601717798201</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="37">
         <v>63.980400000000003</v>
       </c>
-      <c r="H14" s="10">
+      <c r="H14" s="37">
         <v>1.54614206979824</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="37">
         <v>45.5426</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14" s="37">
         <v>0.74817865513525506</v>
       </c>
       <c r="K14">
@@ -1363,433 +1373,433 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="31" t="s">
-        <v>65</v>
+      <c r="A15" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>66</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="10">
-        <v>58.4</v>
-      </c>
-      <c r="E15" s="10">
-        <v>57.26</v>
-      </c>
-      <c r="F15" s="10">
-        <v>1.08535708409721</v>
-      </c>
-      <c r="G15" s="10">
-        <v>72.256199999999893</v>
-      </c>
-      <c r="H15" s="10">
-        <v>1.2930594340555199</v>
-      </c>
-      <c r="I15" s="10">
-        <v>47.868600000000001</v>
-      </c>
-      <c r="J15" s="10">
-        <v>1.47987273101439</v>
+      <c r="D15" s="37">
+        <v>77.2</v>
+      </c>
+      <c r="E15" s="37">
+        <v>76.260000000000005</v>
+      </c>
+      <c r="F15" s="37">
+        <v>0.70922492905988399</v>
+      </c>
+      <c r="G15" s="37">
+        <v>85.985799999999998</v>
+      </c>
+      <c r="H15" s="37">
+        <v>0.72564571245202003</v>
+      </c>
+      <c r="I15" s="37">
+        <v>69.178799999999995</v>
+      </c>
+      <c r="J15" s="37">
+        <v>0.72436986408878201</v>
       </c>
       <c r="K15">
-        <v>1.3657357692718499</v>
+        <v>1.60367751121521</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="31"/>
-      <c r="B16" s="31"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
       <c r="C16" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="5">
-        <v>56.7</v>
-      </c>
-      <c r="E16" s="5">
-        <v>55.18</v>
-      </c>
-      <c r="F16" s="5">
-        <v>0.96020831073262403</v>
-      </c>
-      <c r="G16" s="5">
-        <v>67.563800000000001</v>
-      </c>
-      <c r="H16" s="5">
-        <v>0.71372312558862405</v>
-      </c>
-      <c r="I16" s="5">
-        <v>47.3874</v>
-      </c>
-      <c r="J16" s="5">
-        <v>1.19427919683799</v>
+      <c r="D16" s="37">
+        <v>90.9</v>
+      </c>
+      <c r="E16" s="37">
+        <v>90.26</v>
+      </c>
+      <c r="F16" s="37">
+        <v>0.40373258476372997</v>
+      </c>
+      <c r="G16" s="37">
+        <v>94.796199999999999</v>
+      </c>
+      <c r="H16" s="37">
+        <v>0.51762264247228995</v>
+      </c>
+      <c r="I16" s="37">
+        <v>86.975399999999993</v>
+      </c>
+      <c r="J16" s="37">
+        <v>0.65061724539086296</v>
       </c>
       <c r="K16">
-        <v>1.60367751121521</v>
+        <v>1.7818300724029501</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="31" t="s">
-        <v>64</v>
+      <c r="A17" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>65</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="5">
-        <v>38.9</v>
-      </c>
-      <c r="E17" s="5">
-        <v>37.22</v>
-      </c>
-      <c r="F17" s="5">
-        <v>1.0686440005914</v>
-      </c>
-      <c r="G17" s="5">
-        <v>51.620199999999997</v>
-      </c>
-      <c r="H17" s="5">
-        <v>1.1540722247762401</v>
-      </c>
-      <c r="I17" s="5">
-        <v>27.488399999999999</v>
-      </c>
-      <c r="J17" s="5">
-        <v>1.1543395514318999</v>
+      <c r="D17" s="37">
+        <v>58.4</v>
+      </c>
+      <c r="E17" s="37">
+        <v>57.26</v>
+      </c>
+      <c r="F17" s="37">
+        <v>1.08535708409721</v>
+      </c>
+      <c r="G17" s="37">
+        <v>72.256199999999893</v>
+      </c>
+      <c r="H17" s="37">
+        <v>1.2930594340555199</v>
+      </c>
+      <c r="I17" s="37">
+        <v>47.868600000000001</v>
+      </c>
+      <c r="J17" s="37">
+        <v>1.47987273101439</v>
       </c>
       <c r="K17">
-        <v>2.1663551330566402</v>
+        <v>1.3657357692718499</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="31"/>
-      <c r="B18" s="31"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="5">
-        <v>33.5</v>
-      </c>
-      <c r="E18" s="5">
-        <v>31.98</v>
-      </c>
-      <c r="F18" s="5">
-        <v>1.55788317918899</v>
-      </c>
-      <c r="G18" s="5">
-        <v>43.947400000000002</v>
-      </c>
-      <c r="H18" s="5">
-        <v>1.68619758628696</v>
-      </c>
-      <c r="I18" s="5">
-        <v>23.8964</v>
-      </c>
-      <c r="J18" s="5">
-        <v>1.7732750209710799</v>
+      <c r="D18" s="37">
+        <v>56.7</v>
+      </c>
+      <c r="E18" s="37">
+        <v>55.18</v>
+      </c>
+      <c r="F18" s="37">
+        <v>0.96020831073262403</v>
+      </c>
+      <c r="G18" s="37">
+        <v>67.563800000000001</v>
+      </c>
+      <c r="H18" s="37">
+        <v>0.71372312558862405</v>
+      </c>
+      <c r="I18" s="37">
+        <v>47.3874</v>
+      </c>
+      <c r="J18" s="37">
+        <v>1.19427919683799</v>
       </c>
       <c r="K18">
-        <v>1.89097452163696</v>
+        <v>1.60367751121521</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="B19" s="31" t="s">
-        <v>73</v>
+      <c r="A19" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>63</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="5">
-        <v>74.5</v>
-      </c>
-      <c r="E19" s="5">
-        <v>74.239999999999995</v>
-      </c>
-      <c r="F19" s="5">
-        <v>0.19493588689617899</v>
-      </c>
-      <c r="G19" s="5">
-        <v>83.453599999999994</v>
-      </c>
-      <c r="H19" s="5">
-        <v>0.73452794364816199</v>
-      </c>
-      <c r="I19" s="5">
-        <v>66.810199999999995</v>
-      </c>
-      <c r="J19" s="5">
-        <v>0.98428537528503401</v>
+      <c r="D19" s="37">
+        <v>84.9</v>
+      </c>
+      <c r="E19" s="37">
+        <v>84.38</v>
+      </c>
+      <c r="F19" s="37">
+        <v>0.60580524923443901</v>
+      </c>
+      <c r="G19" s="37">
+        <v>91.994799999999998</v>
+      </c>
+      <c r="H19" s="37">
+        <v>0.32532015000611603</v>
+      </c>
+      <c r="I19" s="37">
+        <v>78.695599999999999</v>
+      </c>
+      <c r="J19" s="37">
+        <v>0.89229132014157997</v>
       </c>
       <c r="K19">
-        <v>0.34156870841979903</v>
+        <v>1.18545246124267</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="31"/>
-      <c r="B20" s="31"/>
+      <c r="A20" s="23"/>
+      <c r="B20" s="23"/>
       <c r="C20" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="5">
-        <v>81.8</v>
-      </c>
-      <c r="E20" s="5">
-        <v>81.28</v>
-      </c>
-      <c r="F20" s="5">
-        <v>0.55407580708780102</v>
-      </c>
-      <c r="G20" s="5">
-        <v>88.380399999999995</v>
-      </c>
-      <c r="H20" s="5">
-        <v>0.662934612160203</v>
-      </c>
-      <c r="I20" s="5">
-        <v>75.5852</v>
-      </c>
-      <c r="J20" s="5">
-        <v>1.56171418639903</v>
+      <c r="D20" s="37">
+        <v>84.9</v>
+      </c>
+      <c r="E20" s="37">
+        <v>84.38</v>
+      </c>
+      <c r="F20" s="37">
+        <v>0.60580524923443901</v>
+      </c>
+      <c r="G20" s="37">
+        <v>91.994799999999998</v>
+      </c>
+      <c r="H20" s="37">
+        <v>0.32532015000611603</v>
+      </c>
+      <c r="I20" s="37">
+        <v>78.695599999999999</v>
+      </c>
+      <c r="J20" s="37">
+        <v>0.89229132014157997</v>
       </c>
       <c r="K20">
-        <v>0.37186455726623502</v>
+        <v>1.33258581161499</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" s="31" t="s">
-        <v>67</v>
+      <c r="A21" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>70</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="5">
-        <v>73.400000000000006</v>
-      </c>
-      <c r="E21" s="5">
-        <v>72.2</v>
-      </c>
-      <c r="F21" s="5">
-        <v>0.79372539331937897</v>
-      </c>
-      <c r="G21" s="5">
-        <v>82.552599999999998</v>
-      </c>
-      <c r="H21" s="5">
-        <v>0.79064423099141201</v>
-      </c>
-      <c r="I21" s="5">
-        <v>65.098600000000005</v>
-      </c>
-      <c r="J21" s="5">
-        <v>1.35300805614748</v>
+      <c r="D21" s="37">
+        <v>42</v>
+      </c>
+      <c r="E21" s="37">
+        <v>41.7</v>
+      </c>
+      <c r="F21" s="37">
+        <v>0.367423461417476</v>
+      </c>
+      <c r="G21" s="37">
+        <v>52.542999999999999</v>
+      </c>
+      <c r="H21" s="37">
+        <v>1.12343936195951</v>
+      </c>
+      <c r="I21" s="37">
+        <v>34.295000000000002</v>
+      </c>
+      <c r="J21" s="37">
+        <v>0.30798782443466599</v>
       </c>
       <c r="K21">
-        <v>0.79655838012695301</v>
+        <v>1.04804134368896</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="31"/>
-      <c r="B22" s="31"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="23"/>
       <c r="C22" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="5">
-        <v>50.8</v>
-      </c>
-      <c r="E22" s="5">
-        <v>49.76</v>
-      </c>
-      <c r="F22" s="5">
-        <v>0.86486993241758403</v>
-      </c>
-      <c r="G22" s="5">
-        <v>61.095399999999998</v>
-      </c>
-      <c r="H22" s="5">
-        <v>1.4872936159346599</v>
-      </c>
-      <c r="I22" s="5">
-        <v>41.952199999999998</v>
-      </c>
-      <c r="J22" s="5">
-        <v>0.84948937603715002</v>
+      <c r="D22" s="37">
+        <v>25.6</v>
+      </c>
+      <c r="E22" s="37">
+        <v>24.64</v>
+      </c>
+      <c r="F22" s="37">
+        <v>0.832466215530696</v>
+      </c>
+      <c r="G22" s="37">
+        <v>35.057000000000002</v>
+      </c>
+      <c r="H22" s="37">
+        <v>1.72089453482774</v>
+      </c>
+      <c r="I22" s="37">
+        <v>17.461600000000001</v>
+      </c>
+      <c r="J22" s="37">
+        <v>0.35255680393377598</v>
       </c>
       <c r="K22">
-        <v>0.723840951919555</v>
+        <v>0.81218218803405695</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" s="31" t="s">
-        <v>66</v>
+      <c r="A23" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>67</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="5">
-        <v>77.2</v>
-      </c>
-      <c r="E23" s="5">
-        <v>76.260000000000005</v>
-      </c>
-      <c r="F23" s="5">
-        <v>0.70922492905988399</v>
-      </c>
-      <c r="G23" s="5">
-        <v>85.985799999999998</v>
-      </c>
-      <c r="H23" s="5">
-        <v>0.72564571245202003</v>
-      </c>
-      <c r="I23" s="5">
-        <v>69.178799999999995</v>
-      </c>
-      <c r="J23" s="5">
-        <v>0.72436986408878201</v>
+      <c r="D23" s="37">
+        <v>73.400000000000006</v>
+      </c>
+      <c r="E23" s="37">
+        <v>72.2</v>
+      </c>
+      <c r="F23" s="37">
+        <v>0.79372539331937897</v>
+      </c>
+      <c r="G23" s="37">
+        <v>82.552599999999998</v>
+      </c>
+      <c r="H23" s="37">
+        <v>0.79064423099141201</v>
+      </c>
+      <c r="I23" s="37">
+        <v>65.098600000000005</v>
+      </c>
+      <c r="J23" s="37">
+        <v>1.35300805614748</v>
       </c>
       <c r="K23">
-        <v>1.60367751121521</v>
+        <v>0.79655838012695301</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="23"/>
       <c r="C24" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D24" s="5">
-        <v>90.9</v>
-      </c>
-      <c r="E24" s="5">
-        <v>90.26</v>
-      </c>
-      <c r="F24" s="5">
-        <v>0.40373258476372997</v>
-      </c>
-      <c r="G24" s="5">
-        <v>94.796199999999999</v>
-      </c>
-      <c r="H24" s="5">
-        <v>0.51762264247228995</v>
-      </c>
-      <c r="I24" s="5">
-        <v>86.975399999999993</v>
-      </c>
-      <c r="J24" s="5">
-        <v>0.65061724539086296</v>
+      <c r="D24" s="37">
+        <v>50.8</v>
+      </c>
+      <c r="E24" s="37">
+        <v>49.76</v>
+      </c>
+      <c r="F24" s="37">
+        <v>0.86486993241758403</v>
+      </c>
+      <c r="G24" s="37">
+        <v>61.095399999999998</v>
+      </c>
+      <c r="H24" s="37">
+        <v>1.4872936159346599</v>
+      </c>
+      <c r="I24" s="37">
+        <v>41.952199999999998</v>
+      </c>
+      <c r="J24" s="37">
+        <v>0.84948937603715002</v>
       </c>
       <c r="K24">
-        <v>1.7818300724029501</v>
+        <v>0.723840951919555</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="31" t="s">
-        <v>63</v>
+      <c r="A25" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>64</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="5">
-        <v>84.9</v>
-      </c>
-      <c r="E25" s="5">
-        <v>84.38</v>
-      </c>
-      <c r="F25" s="5">
-        <v>0.60580524923443901</v>
-      </c>
-      <c r="G25" s="5">
-        <v>91.994799999999998</v>
-      </c>
-      <c r="H25" s="5">
-        <v>0.32532015000611603</v>
-      </c>
-      <c r="I25" s="5">
-        <v>78.695599999999999</v>
-      </c>
-      <c r="J25" s="5">
-        <v>0.89229132014157997</v>
+      <c r="D25" s="37">
+        <v>38.9</v>
+      </c>
+      <c r="E25" s="37">
+        <v>37.22</v>
+      </c>
+      <c r="F25" s="37">
+        <v>1.0686440005914</v>
+      </c>
+      <c r="G25" s="37">
+        <v>51.620199999999997</v>
+      </c>
+      <c r="H25" s="37">
+        <v>1.1540722247762401</v>
+      </c>
+      <c r="I25" s="37">
+        <v>27.488399999999999</v>
+      </c>
+      <c r="J25" s="37">
+        <v>1.1543395514318999</v>
       </c>
       <c r="K25">
-        <v>1.18545246124267</v>
+        <v>2.1663551330566402</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="31"/>
-      <c r="B26" s="31"/>
+      <c r="A26" s="23"/>
+      <c r="B26" s="23"/>
       <c r="C26" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D26" s="5">
-        <v>84.9</v>
-      </c>
-      <c r="E26" s="5">
-        <v>84.38</v>
-      </c>
-      <c r="F26" s="5">
-        <v>0.60580524923443901</v>
-      </c>
-      <c r="G26" s="5">
-        <v>91.994799999999998</v>
-      </c>
-      <c r="H26" s="5">
-        <v>0.32532015000611603</v>
-      </c>
-      <c r="I26" s="5">
-        <v>78.695599999999999</v>
-      </c>
-      <c r="J26" s="5">
-        <v>0.89229132014157997</v>
+      <c r="D26" s="37">
+        <v>33.5</v>
+      </c>
+      <c r="E26" s="37">
+        <v>31.98</v>
+      </c>
+      <c r="F26" s="37">
+        <v>1.55788317918899</v>
+      </c>
+      <c r="G26" s="37">
+        <v>43.947400000000002</v>
+      </c>
+      <c r="H26" s="37">
+        <v>1.68619758628696</v>
+      </c>
+      <c r="I26" s="37">
+        <v>23.8964</v>
+      </c>
+      <c r="J26" s="37">
+        <v>1.7732750209710799</v>
       </c>
       <c r="K26">
-        <v>1.33258581161499</v>
+        <v>1.89097452163696</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A17:A18"/>
     <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:J1"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="B23:B24"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
     <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B16"/>
     <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B25:B26"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -10475,46 +10485,46 @@
     <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" s="17"/>
       <c r="B1" s="17"/>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="25" t="s">
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="27" t="s">
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="25" t="s">
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="32"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -10523,73 +10533,73 @@
       <c r="B2" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23" t="s">
+      <c r="D2" s="31"/>
+      <c r="E2" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23" t="s">
+      <c r="F2" s="31"/>
+      <c r="G2" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23" t="s">
+      <c r="H2" s="31"/>
+      <c r="I2" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="23"/>
-      <c r="K2" s="26" t="s">
+      <c r="J2" s="31"/>
+      <c r="K2" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26" t="s">
+      <c r="L2" s="33"/>
+      <c r="M2" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26" t="s">
+      <c r="N2" s="33"/>
+      <c r="O2" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26" t="s">
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="R2" s="26"/>
-      <c r="S2" s="23" t="s">
+      <c r="R2" s="33"/>
+      <c r="S2" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="23"/>
-      <c r="U2" s="23" t="s">
+      <c r="T2" s="31"/>
+      <c r="U2" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="V2" s="23"/>
-      <c r="W2" s="23" t="s">
+      <c r="V2" s="31"/>
+      <c r="W2" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="23" t="s">
+      <c r="X2" s="31"/>
+      <c r="Y2" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="23"/>
-      <c r="AA2" s="26" t="s">
+      <c r="Z2" s="31"/>
+      <c r="AA2" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="AB2" s="26"/>
-      <c r="AC2" s="26" t="s">
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="AD2" s="26"/>
-      <c r="AE2" s="26" t="s">
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="AF2" s="26"/>
-      <c r="AG2" s="26" t="s">
+      <c r="AF2" s="33"/>
+      <c r="AG2" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="AH2" s="26"/>
+      <c r="AH2" s="33"/>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="35" t="s">
         <v>48</v>
       </c>
       <c r="B3" s="15" t="s">
@@ -10693,7 +10703,7 @@
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A4" s="22"/>
+      <c r="A4" s="35"/>
       <c r="B4" s="15" t="s">
         <v>47</v>
       </c>
@@ -10795,7 +10805,7 @@
       </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="35" t="s">
         <v>49</v>
       </c>
       <c r="B5" s="15" t="s">
@@ -10899,7 +10909,7 @@
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A6" s="22"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="15" t="s">
         <v>47</v>
       </c>
@@ -11001,7 +11011,7 @@
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="35" t="s">
         <v>50</v>
       </c>
       <c r="B7" s="15" t="s">
@@ -11105,7 +11115,7 @@
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A8" s="22"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="15" t="s">
         <v>47</v>
       </c>
@@ -11207,7 +11217,7 @@
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="35" t="s">
         <v>51</v>
       </c>
       <c r="B9" s="15" t="s">
@@ -11311,7 +11321,7 @@
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A10" s="22"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="15" t="s">
         <v>47</v>
       </c>
@@ -11413,7 +11423,7 @@
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="35" t="s">
         <v>53</v>
       </c>
       <c r="B11" s="15" t="s">
@@ -11517,7 +11527,7 @@
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A12" s="22"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="15" t="s">
         <v>47</v>
       </c>
@@ -11619,7 +11629,7 @@
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="35" t="s">
         <v>52</v>
       </c>
       <c r="B13" s="15" t="s">
@@ -11723,7 +11733,7 @@
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="15" t="s">
         <v>47</v>
       </c>
@@ -11825,7 +11835,7 @@
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="35" t="s">
         <v>54</v>
       </c>
       <c r="B15" s="15" t="s">
@@ -11929,7 +11939,7 @@
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A16" s="22"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="15" t="s">
         <v>47</v>
       </c>
@@ -12031,7 +12041,7 @@
       </c>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="35" t="s">
         <v>55</v>
       </c>
       <c r="B17" s="15" t="s">
@@ -12135,7 +12145,7 @@
       </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A18" s="22"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="15" t="s">
         <v>47</v>
       </c>
@@ -12241,23 +12251,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="S1:Z1"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AA1:AH1"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="C1:J1"/>
-    <mergeCell ref="K1:R1"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="I2:J2"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="C2:D2"/>
@@ -12269,6 +12262,23 @@
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="K1:R1"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="AA1:AH1"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="S1:Z1"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="Y2:Z2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -21039,38 +21049,38 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29" t="s">
+      <c r="F2" s="24"/>
+      <c r="G2" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29" t="s">
+      <c r="H2" s="24"/>
+      <c r="I2" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="29"/>
+      <c r="J2" s="24"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
@@ -21635,38 +21645,38 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29" t="s">
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="F24" s="29"/>
-      <c r="G24" s="29" t="s">
+      <c r="F24" s="24"/>
+      <c r="G24" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="H24" s="29"/>
-      <c r="I24" s="29" t="s">
+      <c r="H24" s="24"/>
+      <c r="I24" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="J24" s="29"/>
+      <c r="J24" s="24"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
@@ -29130,25 +29140,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
       <c r="G1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.35">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
       <c r="C2" s="8">
         <v>5</v>
       </c>
@@ -29166,7 +29176,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="23" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -29189,7 +29199,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="31"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
@@ -29207,7 +29217,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="23" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -29227,7 +29237,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="31"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="6" t="s">
         <v>1</v>
       </c>
@@ -29245,7 +29255,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="23" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -29265,7 +29275,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="31"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="6" t="s">
         <v>1</v>
       </c>
@@ -29283,7 +29293,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="23" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -29303,7 +29313,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="31"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="6" t="s">
         <v>1</v>
       </c>
@@ -29321,22 +29331,22 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="30"/>
-      <c r="B13" s="30"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
       <c r="C13" s="8">
         <v>5</v>
       </c>
@@ -29349,12 +29359,12 @@
       <c r="F13" s="8">
         <v>8</v>
       </c>
-      <c r="G13" s="34">
+      <c r="G13" s="22">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="23" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -29374,7 +29384,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="31"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="6" t="s">
         <v>1</v>
       </c>
@@ -29392,7 +29402,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="23" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="6" t="s">
@@ -29412,7 +29422,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="31"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="6" t="s">
         <v>1</v>
       </c>
@@ -29430,7 +29440,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="6" t="s">
@@ -29450,7 +29460,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="31"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="6" t="s">
         <v>1</v>
       </c>
@@ -29468,7 +29478,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B20" s="6" t="s">
@@ -29488,7 +29498,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="31"/>
+      <c r="A21" s="23"/>
       <c r="B21" s="6" t="s">
         <v>1</v>
       </c>
@@ -29506,7 +29516,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="23" t="s">
         <v>6</v>
       </c>
       <c r="B22" s="6" t="s">
@@ -29526,7 +29536,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="31"/>
+      <c r="A23" s="23"/>
       <c r="B23" s="6" t="s">
         <v>1</v>
       </c>
@@ -29544,7 +29554,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="23" t="s">
         <v>5</v>
       </c>
       <c r="B24" s="6" t="s">
@@ -29564,7 +29574,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="31"/>
+      <c r="A25" s="23"/>
       <c r="B25" s="6" t="s">
         <v>1</v>
       </c>
@@ -29582,7 +29592,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="23" t="s">
         <v>4</v>
       </c>
       <c r="B26" s="6" t="s">
@@ -29605,7 +29615,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="31"/>
+      <c r="A27" s="23"/>
       <c r="B27" s="6" t="s">
         <v>1</v>
       </c>
@@ -29626,7 +29636,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="23" t="s">
         <v>3</v>
       </c>
       <c r="B28" s="6" t="s">
@@ -29646,7 +29656,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="31"/>
+      <c r="A29" s="23"/>
       <c r="B29" s="6" t="s">
         <v>1</v>
       </c>
@@ -29665,6 +29675,17 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A26:A27"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>
@@ -29672,17 +29693,6 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>